<commit_message>
chore: remove invoice feature; fix monthly export weekly sheets + admin cache-bust
</commit_message>
<xml_diff>
--- a/labor-timekeeper/exports/2025-12/2025-12-29/Chris_Jacobi_2025-12-29.xlsx
+++ b/labor-timekeeper/exports/2025-12/2025-12-29/Chris_Jacobi_2025-12-29.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -31,19 +31,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2026-01-01</t>
-  </si>
-  <si>
-    <t>Campbell</t>
-  </si>
-  <si>
-    <t>Holiday</t>
-  </si>
-  <si>
     <t>2026-01-02</t>
   </si>
   <si>
-    <t>Schneebeck</t>
+    <t>Ueltschi</t>
   </si>
   <si>
     <t>Regular</t>
@@ -55,7 +46,7 @@
     <t/>
   </si>
   <si>
-    <t>Reg: 18 / OT: 0</t>
+    <t>Reg: 6.5 / OT: 0</t>
   </si>
   <si>
     <t>Category: ADMIN</t>
@@ -456,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -495,76 +486,56 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1">
-        <v>900</v>
+        <v>552.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1">
-        <v>900</v>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>552.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>